<commit_message>
Add link to CONTRIBUTING
</commit_message>
<xml_diff>
--- a/google_nq/expe/04. Evals/ready_to_gen_facts_google_nq--30Q_0C_221F_1M_30A_30HE_30AE_2024-04-01_00h50,33.xlsx
+++ b/google_nq/expe/04. Evals/ready_to_gen_facts_google_nq--30Q_0C_221F_1M_30A_30HE_30AE_2024-04-01_00h50,33.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gilles_recital\source\repos\rag-projects\google_nq\expe\04. Evals\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B281D876-A5DA-45BA-9D24-73EE0EBD6F3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2536E053-86B4-49BA-A3C3-4D1A11CCDB08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2039,7 +2039,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
+      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelCol="1" x14ac:dyDescent="0.3"/>

</xml_diff>